<commit_message>
Updated BOM with new speaker, and lower value LED ring resistor.
</commit_message>
<xml_diff>
--- a/MAG Synth/BOM/Stylish-Belt-Synth - Full.xlsx
+++ b/MAG Synth/BOM/Stylish-Belt-Synth - Full.xlsx
@@ -13,14 +13,14 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="107">
   <si>
     <t xml:space="preserve">Stylish! Trucker Belt Buckle Synthesizer</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changed</t>
   </si>
   <si>
     <t xml:space="preserve">R4</t>
@@ -221,16 +224,43 @@
     <t xml:space="preserve">LS1</t>
   </si>
   <si>
-    <t xml:space="preserve">Pin_Header_Angle_1x02_Pitch2.54mm</t>
+    <t xml:space="preserve">4 Ohm 3W Loudspeaker 52MM</t>
   </si>
   <si>
     <t xml:space="preserve">Speaker</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.aliexpress.com/item/32907473925.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Speaker will mount in center hole. Leads should be long enough to reach and leave some slack.</t>
+    <t xml:space="preserve">https://www.aliexpress.com/item/32710566874.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speaker will mount in center hole. Leads should be long enough to reach and leave some slack. </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>July 12</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, 2019</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">CA4</t>
@@ -281,10 +311,37 @@
     <t xml:space="preserve">R3</t>
   </si>
   <si>
-    <t xml:space="preserve">44Ω</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43Ω is ok.</t>
+    <t xml:space="preserve">30Ω</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lowered to improve LED blue and green color.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>July 13</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, 2019</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">U1</t>
@@ -358,7 +415,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -401,16 +458,28 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -432,6 +501,20 @@
       <bottom style="hair"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -458,7 +541,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -467,6 +550,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -479,6 +566,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -491,27 +582,115 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -534,8 +713,8 @@
   </sheetPr>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.65"/>
@@ -544,563 +723,613 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.5867346938776"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.22448979591837"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.4795918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.1581632653061"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41.1632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="12.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" s="3" customFormat="true" ht="26.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+    <row r="2" s="4" customFormat="true" ht="26.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" s="8" customFormat="true" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+    <row r="4" s="11" customFormat="true" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="0"/>
+      <c r="G4" s="10" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="10" t="s">
+      <c r="A5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="11" t="s">
+      <c r="B5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="C5" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="12"/>
+      <c r="E5" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="15"/>
+      <c r="G5" s="16"/>
     </row>
     <row r="6" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="11" t="s">
+      <c r="A6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="B6" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="12"/>
+      <c r="E6" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="20"/>
+      <c r="G6" s="21"/>
     </row>
     <row r="7" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="12"/>
-    </row>
-    <row r="8" customFormat="false" ht="28.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="10" t="s">
+      <c r="F7" s="25"/>
+      <c r="G7" s="26"/>
+    </row>
+    <row r="8" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="11" t="s">
+      <c r="B8" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="C8" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="E8" s="18" t="s">
         <v>22</v>
       </c>
+      <c r="F8" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="10" t="s">
+      <c r="A9" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="11" t="n">
+      <c r="B9" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="12" t="s">
+      <c r="D9" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="12"/>
+      <c r="E9" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="25"/>
+      <c r="G9" s="26"/>
     </row>
     <row r="10" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" s="11" t="s">
+      <c r="A10" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="12"/>
+      <c r="B10" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="27"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" customFormat="false" ht="17.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="10" t="s">
+      <c r="A11" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" s="11" t="s">
+      <c r="B11" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
+      <c r="C11" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="26"/>
     </row>
     <row r="12" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="10" t="s">
+      <c r="A12" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="11" t="n">
+      <c r="B12" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="12" t="s">
+      <c r="D12" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="E12" s="27" t="s">
         <v>36</v>
       </c>
+      <c r="F12" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="21"/>
     </row>
     <row r="13" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="11" t="n">
+      <c r="A13" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="12" t="s">
+      <c r="D13" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="E13" s="25" t="s">
         <v>40</v>
       </c>
+      <c r="F13" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="26"/>
     </row>
     <row r="14" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="10" t="s">
+      <c r="A14" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D14" s="11" t="s">
+      <c r="B14" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="C14" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="12"/>
+      <c r="E14" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="27"/>
+      <c r="G14" s="21"/>
     </row>
     <row r="15" customFormat="false" ht="95.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="10" t="s">
+      <c r="A15" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="11" t="n">
+      <c r="B15" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="24" t="n">
         <v>16</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="12" t="s">
+      <c r="D15" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="E15" s="25" t="s">
         <v>48</v>
       </c>
+      <c r="F15" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="26"/>
     </row>
     <row r="16" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D16" s="11" t="s">
+      <c r="A16" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="B16" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="F16" s="12"/>
-    </row>
-    <row r="17" customFormat="false" ht="28.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9" t="s">
+      <c r="E16" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="F16" s="27"/>
+      <c r="G16" s="21"/>
+    </row>
+    <row r="17" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D17" s="11" t="s">
+      <c r="B17" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="C17" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="E17" s="25" t="s">
         <v>56</v>
       </c>
+      <c r="F17" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="26"/>
     </row>
     <row r="18" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" s="10" t="s">
+      <c r="G18" s="21"/>
+    </row>
+    <row r="19" s="33" customFormat="true" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D19" s="11" t="s">
+      <c r="B19" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="C19" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="E19" s="28" t="s">
         <v>64</v>
       </c>
+      <c r="F19" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" s="32" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="12" t="s">
+      <c r="A20" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="F20" s="12"/>
+      <c r="B20" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="27"/>
+      <c r="G20" s="21"/>
     </row>
     <row r="21" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" s="12" t="s">
+      <c r="A21" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="B21" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="24" t="s">
         <v>71</v>
       </c>
+      <c r="E21" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="G21" s="26"/>
     </row>
     <row r="22" customFormat="false" ht="72.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C22" s="11" t="n">
+      <c r="A22" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="19" t="n">
         <v>16</v>
       </c>
-      <c r="D22" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="F22" s="12"/>
+      <c r="D22" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="27"/>
+      <c r="G22" s="21"/>
     </row>
     <row r="23" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F23" s="12"/>
+      <c r="A23" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="25"/>
+      <c r="G23" s="26"/>
     </row>
     <row r="24" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F24" s="12"/>
-    </row>
-    <row r="25" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="9" t="s">
+      <c r="A24" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="B25" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D25" s="11" t="s">
+      <c r="B24" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="E25" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F25" s="12" t="s">
+      <c r="E24" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" s="27"/>
+      <c r="G24" s="21"/>
+    </row>
+    <row r="25" s="33" customFormat="true" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="28" t="s">
         <v>82</v>
       </c>
+      <c r="B25" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="G25" s="32" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="72.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C26" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E26" s="12" t="s">
+      <c r="A26" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="B26" s="18" t="s">
         <v>87</v>
       </c>
+      <c r="C26" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="G26" s="21"/>
     </row>
     <row r="27" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B27" s="10" t="s">
+      <c r="A27" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="D27" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="C27" s="11" t="n">
+      <c r="E27" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="F27" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="G27" s="26"/>
+    </row>
+    <row r="28" customFormat="false" ht="50.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E28" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="F28" s="27"/>
+      <c r="G28" s="21"/>
+    </row>
+    <row r="29" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C29" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="F29" s="25"/>
+      <c r="G29" s="26"/>
+    </row>
+    <row r="30" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="35"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="21"/>
+    </row>
+    <row r="31" s="37" customFormat="true" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="F31" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="G31" s="22"/>
+    </row>
+    <row r="32" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="C32" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="D27" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="50.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="C28" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="F28" s="12"/>
-    </row>
-    <row r="29" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C29" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="F29" s="12"/>
-    </row>
-    <row r="31" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="C31" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="C32" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="F32" s="0" t="s">
-        <v>103</v>
-      </c>
+      <c r="D32" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="G32" s="21"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F15" r:id="rId1" display="http://www.world-semi.com/DownLoadFile/108"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>